<commit_message>
fixed bugs and update on RC excel label printing
</commit_message>
<xml_diff>
--- a/DeliveryOrder-92242.xlsx
+++ b/DeliveryOrder-92242.xlsx
@@ -12,7 +12,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>PO Number:</t>
+  </si>
+  <si>
+    <t>9018</t>
+  </si>
+  <si>
+    <t>DO Number:</t>
+  </si>
+  <si>
+    <t>92242</t>
+  </si>
+  <si>
+    <t>Delivery Dater:</t>
+  </si>
+  <si>
+    <t>2021-08-05</t>
+  </si>
+  <si>
+    <t>Company:</t>
+  </si>
+  <si>
+    <t>UBUNTU</t>
+  </si>
+  <si>
+    <t>Courier:</t>
+  </si>
+  <si>
+    <t>FedEx</t>
+  </si>
   <si>
     <t>SN</t>
   </si>
@@ -89,43 +119,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.8671875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="7.7265625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.4375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.3046875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="22.640625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.94921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>1.0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>